<commit_message>
added images and previous screening to Screening Assessment
</commit_message>
<xml_diff>
--- a/db/support/cbdmat_markers.xlsx
+++ b/db/support/cbdmat_markers.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://childreninfamilies-my.sharepoint.com/personal/meas_kiry_childreninfamilies_org/Documents/Microsoft Teams Chat Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\kiry\Documents\oscar-web\db\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_98EC1EEF06F20B30981045321473C1EEC7FDF072" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E001F23E-F354-4763-8702-CD83DD4BD160}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69F10BC-3590-4D41-915B-960D1AD62AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="6720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="6 moths_៦ ខែ" sheetId="1" r:id="rId1"/>
+    <sheet name="6 months_៦ ខែ" sheetId="1" r:id="rId1"/>
     <sheet name="9 months_៩ ខែ" sheetId="2" r:id="rId2"/>
     <sheet name="1 year_១ ឆ្នាំ" sheetId="3" r:id="rId3"/>
     <sheet name="1.5 years_១ ឆ្នាំកន្លះ" sheetId="4" r:id="rId4"/>
@@ -753,7 +753,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -763,7 +763,7 @@
     <col min="3" max="3" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -774,7 +774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -783,7 +783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1335,7 +1335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>